<commit_message>
excel recalculate total and re-write the file
</commit_message>
<xml_diff>
--- a/store.xlsx
+++ b/store.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2091" yWindow="2091" windowWidth="30446" windowHeight="14700" tabRatio="991" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6094" yWindow="2537" windowWidth="22063" windowHeight="14700" tabRatio="991" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" state="visible" r:id="rId1"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="17.6"/>

</xml_diff>

<commit_message>
CRUD operations with sheet
</commit_message>
<xml_diff>
--- a/store.xlsx
+++ b/store.xlsx
@@ -6,8 +6,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6094" yWindow="2537" windowWidth="22063" windowHeight="14700" tabRatio="991" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Products" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sales 2018" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NewSheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Products" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sales 2018" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="NewSheet1 Copy" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -491,6 +493,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -761,7 +781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -920,4 +940,22 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>